<commit_message>
Exception Handling examples 23-01-2024
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java FSD 28th Dec 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java Fsd 12 th 2023 Dec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DDBA68-B866-409A-9AB2-6504CF6AEB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2558D46-7450-4807-9DD5-9A6DC0A2EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Updates" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Git Links" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t>Concepts</t>
   </si>
@@ -136,118 +136,124 @@
     <t>introduction</t>
   </si>
   <si>
+    <t>9:30Pm-10:30pm</t>
+  </si>
+  <si>
+    <t>java,.class,compaliation,execution,compiler,overview jdk,jvm,jre</t>
+  </si>
+  <si>
+    <t>9:40Pm-10:30pm</t>
+  </si>
+  <si>
+    <t>Java Installation,eclipse</t>
+  </si>
+  <si>
+    <t>Identifiers,variables,datatypes</t>
+  </si>
+  <si>
+    <t>9:50pm-10:40pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance and static </t>
+  </si>
+  <si>
+    <t>work on assignments  day-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JVM Architecture </t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>https://github.com/RB0896/Full_Stack</t>
+  </si>
+  <si>
+    <t>Gomanth Sainath</t>
+  </si>
+  <si>
     <t>https://docs.oracle.com/javase/8/docs/api/</t>
   </si>
   <si>
-    <t>karthik reddy</t>
-  </si>
-  <si>
-    <t>shiva teja</t>
-  </si>
-  <si>
-    <t>8:00AM-9:00AM</t>
-  </si>
-  <si>
-    <t>Nani</t>
-  </si>
-  <si>
-    <t>https://www.javatpoint.com/javafx-how-to-install-java</t>
-  </si>
-  <si>
-    <t>Java installation,execute hello world example</t>
-  </si>
-  <si>
-    <t>java file,.class file,compailation,execution flow</t>
-  </si>
-  <si>
-    <t>https://github.com/karthikreddykothakapu/javatraining.git</t>
-  </si>
-  <si>
-    <t>https://github.com/Shivateja29/JavaTraining.git</t>
-  </si>
-  <si>
-    <t>https://github.com/Hemanth1818/Java.git</t>
-  </si>
-  <si>
-    <t>identifiers,variables,datatypes</t>
-  </si>
-  <si>
-    <t>complete assignment day-1</t>
-  </si>
-  <si>
-    <t>Agastya Teja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variables instance and static </t>
-  </si>
-  <si>
-    <t>8:30AM-9:06Am</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshik Kumar </t>
-  </si>
-  <si>
-    <t>import,package</t>
-  </si>
-  <si>
-    <t>https://www.eclipse.org/downloads/packages/release/2022-03/r</t>
-  </si>
-  <si>
-    <t>eclipse installation,flow control excercises</t>
-  </si>
-  <si>
-    <t>Flow control statements,eclipse</t>
-  </si>
-  <si>
-    <t>https://github.com/deshik9999/Java</t>
+    <t>https://github.com/GomanthSainath/Assignment-Day1.git</t>
+  </si>
+  <si>
+    <t>Dynamic data,eclipse,package,import,wrapper class</t>
+  </si>
+  <si>
+    <t>Scanner,revision of package and import in eclipse</t>
+  </si>
+  <si>
+    <t>Methods ,instance,static methods</t>
   </si>
   <si>
     <t>flow control statements</t>
   </si>
   <si>
-    <t>Trainer not available(fever)</t>
-  </si>
-  <si>
-    <t>JVM Architecture</t>
-  </si>
-  <si>
-    <t>Operators https://www.w3schools.com/java/java_operators.asp</t>
-  </si>
-  <si>
-    <t>Revision</t>
-  </si>
-  <si>
-    <t>MCQ Quiz and Revision</t>
-  </si>
-  <si>
-    <t>methods</t>
-  </si>
-  <si>
-    <t>Tejesh</t>
-  </si>
-  <si>
-    <t>https://github.com/AgastyaTeja1/JavaTraining</t>
-  </si>
-  <si>
-    <t>https://github.com/tejesh57</t>
-  </si>
-  <si>
-    <t>MethodsAndScannetask day2.docx</t>
-  </si>
-  <si>
-    <t>ArraysAssignment</t>
-  </si>
-  <si>
-    <t>args,Scanner,wrapper classes ,arrays basics</t>
-  </si>
-  <si>
-    <t>OOPS(Inheritance extends,implements)</t>
-  </si>
-  <si>
-    <t>Trainer not available joined late</t>
-  </si>
-  <si>
-    <t>OOPS(abstract methods,concrete methods,abstract class,interface,abstraction)</t>
+    <t>Work on Assignments(Flow Control Exercises,Core java Basics Task.docx)</t>
+  </si>
+  <si>
+    <t>OOPS Intro</t>
+  </si>
+  <si>
+    <t>Inheritance and different levels abstract methods and concrete methods intro</t>
+  </si>
+  <si>
+    <t>Abstract class,interface,class,methods,MI</t>
+  </si>
+  <si>
+    <t>9:45Pm-10:45pm</t>
+  </si>
+  <si>
+    <t>OOPS Task</t>
+  </si>
+  <si>
+    <t>Access modifiers,polymorphisam(Overloading)</t>
+  </si>
+  <si>
+    <t>constructor,this,super</t>
+  </si>
+  <si>
+    <t>Overriding ,final</t>
+  </si>
+  <si>
+    <t>9:30Pm-10:25pm</t>
+  </si>
+  <si>
+    <t>Encapsulation</t>
+  </si>
+  <si>
+    <t>MCQ TEST</t>
+  </si>
+  <si>
+    <t>String tasks</t>
+  </si>
+  <si>
+    <t>String,StringBuffer,StringBuilder</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>9:30Pm-10:55pm</t>
+  </si>
+  <si>
+    <t>MCQ Discussion Test</t>
+  </si>
+  <si>
+    <t>15/30</t>
+  </si>
+  <si>
+    <t>Exception Handling</t>
+  </si>
+  <si>
+    <t>Arrays Assignment.docx</t>
+  </si>
+  <si>
+    <t>Exception Handling Assignment Exceptions Task.docx</t>
+  </si>
+  <si>
+    <t>Overriding with exception handling,covarient return type</t>
   </si>
 </sst>
 </file>
@@ -301,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,12 +329,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,7 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -421,11 +421,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -709,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,13 +752,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="4">
-        <v>45288</v>
+        <v>45272</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="9" t="s">
@@ -775,37 +770,33 @@
         <v>9</v>
       </c>
       <c r="E6" s="4">
-        <v>45289</v>
+        <v>45273</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>41</v>
-      </c>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="4">
-        <v>45293</v>
+        <v>45274</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>48</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
@@ -813,15 +804,17 @@
         <v>11</v>
       </c>
       <c r="E8" s="4">
-        <v>45294</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>50</v>
+        <v>45275</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
@@ -829,17 +822,17 @@
         <v>12</v>
       </c>
       <c r="E9" s="4">
-        <v>45295</v>
+        <v>45278</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
@@ -847,33 +840,29 @@
         <v>13</v>
       </c>
       <c r="E10" s="4">
-        <v>45296</v>
+        <v>45279</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>54</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="4">
-        <v>45299</v>
+        <v>45280</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -883,12 +872,14 @@
         <v>15</v>
       </c>
       <c r="E12" s="4">
-        <v>45300</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>45281</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="9"/>
     </row>
@@ -897,16 +888,16 @@
         <v>16</v>
       </c>
       <c r="E13" s="4">
-        <v>45301</v>
+        <v>45282</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -915,13 +906,13 @@
         <v>17</v>
       </c>
       <c r="E14" s="4">
-        <v>45302</v>
+        <v>45286</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -931,13 +922,13 @@
         <v>18</v>
       </c>
       <c r="E15" s="4">
-        <v>45303</v>
+        <v>45287</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="9"/>
@@ -947,17 +938,15 @@
         <v>19</v>
       </c>
       <c r="E16" s="4">
-        <v>45307</v>
+        <v>45288</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -965,16 +954,16 @@
         <v>20</v>
       </c>
       <c r="E17" s="4">
-        <v>45309</v>
+        <v>45289</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -983,13 +972,13 @@
         <v>21</v>
       </c>
       <c r="E18" s="4">
-        <v>45310</v>
+        <v>45293</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1000,12 +989,14 @@
         <v>22</v>
       </c>
       <c r="E19" s="4">
-        <v>45313</v>
+        <v>45294</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
@@ -1014,13 +1005,13 @@
         <v>23</v>
       </c>
       <c r="E20" s="4">
-        <v>45314</v>
+        <v>45295</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1029,29 +1020,51 @@
       <c r="D21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="3"/>
+      <c r="E21" s="4">
+        <v>45296</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="3"/>
+      <c r="E22" s="4">
+        <v>45301</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="5"/>
+      <c r="E23" s="4">
+        <v>45302</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="9"/>
     </row>
@@ -1059,9 +1072,15 @@
       <c r="D24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="4">
+        <v>45303</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="M24" s="8"/>
@@ -1070,10 +1089,18 @@
       <c r="D25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="3"/>
+      <c r="E25" s="4">
+        <v>45309</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="M25" s="8"/>
     </row>
@@ -1081,9 +1108,15 @@
       <c r="D26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="E26" s="4">
+        <v>45310</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="M26" s="8"/>
@@ -1092,19 +1125,33 @@
       <c r="D27" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="E27" s="4">
+        <v>45313</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="4">
+        <v>45314</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
@@ -2148,19 +2195,18 @@
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" xr:uid="{C438D4D9-FF94-4163-9A83-2CC81A380B4A}"/>
     <hyperlink ref="I9" r:id="rId2" xr:uid="{64D4F9BF-372A-4548-B3FA-BC075981D704}"/>
-    <hyperlink ref="I6" r:id="rId3" xr:uid="{DC1A0315-6239-4F78-B007-6C5CA824BB60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="E7:F13"/>
+  <dimension ref="E6:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2169,65 +2215,43 @@
     <col min="6" max="6" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E11" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E13" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>67</v>
-      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{93BB7733-8BF6-4AA3-AC6B-9D4A245EFA49}"/>
-    <hyperlink ref="F9" r:id="rId2" xr:uid="{0FEE7417-566F-4B31-A680-AB6B318BD5E1}"/>
-    <hyperlink ref="F10" r:id="rId3" xr:uid="{CB5E4549-4376-4532-9602-3CA601E2AEE8}"/>
-    <hyperlink ref="F12" r:id="rId4" xr:uid="{4E551DEE-8104-4B2E-B3FF-C56B3F2D44E3}"/>
-    <hyperlink ref="F11" r:id="rId5" xr:uid="{78A9B94E-BF48-4B7B-BE1B-50B73B7B8174}"/>
-    <hyperlink ref="F13" r:id="rId6" xr:uid="{7A6F6C85-B924-4A3C-9031-D69354E53AF7}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{BA4D1F74-267E-4108-A3EC-6863B284671D}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{19397755-44D9-4CAC-961A-54C61207C4B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Exception Handling Examples and notes
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java FSD 28th Dec 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2A88B2-71CC-4EDE-A78F-B2BCA7DDF9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34C6503-C4E9-47C6-8788-B1E8C5D003C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t>Concepts</t>
   </si>
@@ -272,6 +272,27 @@
   </si>
   <si>
     <t>8:00AM-9:15AM</t>
+  </si>
+  <si>
+    <t>8:00AM-9:10AM</t>
+  </si>
+  <si>
+    <t>Exception Handling  Intro</t>
+  </si>
+  <si>
+    <t>8:10AM-9:00AM</t>
+  </si>
+  <si>
+    <t>MCQ TEST</t>
+  </si>
+  <si>
+    <t>Mcq Questions discussion and exception handling</t>
+  </si>
+  <si>
+    <t>String,StringBuffer,StringBuilder</t>
+  </si>
+  <si>
+    <t>Exception Handling  (try,catch,finally,throw,throws)</t>
   </si>
 </sst>
 </file>
@@ -733,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,7 +1131,7 @@
         <v>80</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1123,11 +1144,13 @@
       <c r="E25" s="4">
         <v>45321</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="F25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="M25" s="8"/>
     </row>
@@ -1135,10 +1158,18 @@
       <c r="D26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="E26" s="4">
+        <v>45322</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="M26" s="8"/>
     </row>
@@ -1146,9 +1177,15 @@
       <c r="D27" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="E27" s="4">
+        <v>45323</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
@@ -1156,9 +1193,15 @@
       <c r="D28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="4">
+        <v>45324</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
@@ -1166,9 +1209,15 @@
       <c r="D29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="4">
+        <v>45327</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>

</xml_diff>

<commit_message>
File IO Stream Examples
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java FSD 28th Dec 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374A2D98-40DF-41F3-95E1-D77F78E2AC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02F994-2CDC-4067-BFA4-181E3867ECB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
   <si>
     <t>Concepts</t>
   </si>
@@ -313,7 +313,19 @@
     <t>Day-29</t>
   </si>
   <si>
-    <t>multi threading,thread life cycle,snchronization,inter thread communication and methods</t>
+    <t>multi threading,thread life cycle,snchronization,thread class methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inter thread communication </t>
+  </si>
+  <si>
+    <t>Day-30</t>
+  </si>
+  <si>
+    <t>Day-31</t>
+  </si>
+  <si>
+    <t>File IO TASK</t>
   </si>
 </sst>
 </file>
@@ -775,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1302,26 +1314,46 @@
         <v>45331</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G33" s="10"/>
+        <v>96</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="6"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="10"/>
+      <c r="D34" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="4">
+        <v>45334</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D35" s="6"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="3"/>
+      <c r="D35" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="4">
+        <v>45335</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">

</xml_diff>